<commit_message>
Implementing SequentialSetGeneration from (Gao et al., 2019) A Sequential Set Generation Method for Predicting Set-Valued Outputs
</commit_message>
<xml_diff>
--- a/NTCIR/res.xlsx
+++ b/NTCIR/res.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ygorgallina/Documents/Prog/thesis_workspace/NTCIR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121D8B64-CD28-2E49-8D29-AC5CAA64C17E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F94C6D-0DE8-9E4E-8977-F8E102D126A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{479949D6-3E36-CA4F-AA7D-65811C6EE087}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="55">
   <si>
     <t>Index</t>
   </si>
@@ -39,19 +39,10 @@
     <t>occ ntc2-e1k</t>
   </si>
   <si>
-    <t>freq ntc2-e1k</t>
-  </si>
-  <si>
     <t>occ ntc2-e1g</t>
   </si>
   <si>
-    <t>freq ntc2-e1g</t>
-  </si>
-  <si>
     <t>occ ntc1-e1</t>
-  </si>
-  <si>
-    <t>freq ntc1-e1</t>
   </si>
   <si>
     <t>CopyRNN</t>
@@ -240,8 +231,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -294,11 +286,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-FR"/>
-              <a:t>Location</a:t>
+              <a:t>Percentage</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="fr-FR" baseline="0"/>
-              <a:t> of difference difference between beam size 200 and beam size 50</a:t>
+              <a:t> of difference between output of beam size 200 and beam size 50 per rank</a:t>
             </a:r>
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
@@ -348,7 +340,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>freq ntc2-e1k</c:v>
+                  <c:v>ntc2-e1k</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -538,7 +530,7 @@
             <c:numRef>
               <c:f>Feuil1!$C$3:$C$54</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
                   <c:v>1.2641857442830359E-6</c:v>
@@ -709,7 +701,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>freq ntc1-e1</c:v>
+                  <c:v>ntc1-e1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -899,7 +891,7 @@
             <c:numRef>
               <c:f>Feuil1!$G$3:$G$54</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
                   <c:v>6.2937475312433256E-6</c:v>
@@ -1070,7 +1062,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>freq ntc2-e1g</c:v>
+                  <c:v>ntc2-e1g</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1260,7 +1252,7 @@
             <c:numRef>
               <c:f>Feuil1!$E$3:$E$54</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
                   <c:v>5.976510322263397E-6</c:v>
@@ -1516,7 +1508,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2193,16 +2185,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>82550</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>679450</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2527,13 +2519,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0AB6827-F974-A947-A77D-39C83934718A}">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2542,20 +2539,20 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
+      <c r="G1" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2565,20 +2562,19 @@
       <c r="B2">
         <v>2251393</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>0.94872631179287248</v>
       </c>
       <c r="D2">
         <v>2891035</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>0.9599055844180423</v>
       </c>
       <c r="F2">
         <v>7000332</v>
       </c>
-      <c r="G2">
-        <f>F2/SUM(F:F)</f>
+      <c r="G2" s="1">
         <v>0.95778961397573159</v>
       </c>
     </row>
@@ -2589,20 +2585,19 @@
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>1.2641857442830359E-6</v>
       </c>
       <c r="D3">
         <v>18</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>5.976510322263397E-6</v>
       </c>
       <c r="F3">
         <v>46</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G52" si="0">F3/SUM(F:F)</f>
+      <c r="G3" s="1">
         <v>6.2937475312433256E-6</v>
       </c>
     </row>
@@ -2613,20 +2608,19 @@
       <c r="B4">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>5.0567429771321437E-6</v>
       </c>
       <c r="D4">
         <v>68</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>2.2577927884106166E-5</v>
       </c>
       <c r="F4">
         <v>123</v>
       </c>
-      <c r="G4">
-        <f t="shared" si="0"/>
+      <c r="G4" s="1">
         <v>1.6828933616150632E-5</v>
       </c>
     </row>
@@ -2637,20 +2631,19 @@
       <c r="B5">
         <v>34</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>1.4327438435207741E-5</v>
       </c>
       <c r="D5">
         <v>101</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>3.3534863474922397E-5</v>
       </c>
       <c r="F5">
         <v>233</v>
       </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
+      <c r="G5" s="1">
         <v>3.1879199451732498E-5</v>
       </c>
     </row>
@@ -2661,20 +2654,19 @@
       <c r="B6">
         <v>53</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>2.2333948149000303E-5</v>
       </c>
       <c r="D6">
         <v>116</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>3.8515288743475229E-5</v>
       </c>
       <c r="F6">
         <v>330</v>
       </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
+      <c r="G6" s="1">
         <v>4.5150797506745599E-5</v>
       </c>
     </row>
@@ -2685,20 +2677,19 @@
       <c r="B7">
         <v>71</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>2.9919062614698521E-5</v>
       </c>
       <c r="D7">
         <v>159</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>5.2792507846660008E-5</v>
       </c>
       <c r="F7">
         <v>394</v>
       </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
+      <c r="G7" s="1">
         <v>5.3907315811084136E-5</v>
       </c>
     </row>
@@ -2709,20 +2700,19 @@
       <c r="B8">
         <v>88</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>3.7082781832302392E-5</v>
       </c>
       <c r="D8">
         <v>200</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>6.6405670247371085E-5</v>
       </c>
       <c r="F8">
         <v>453</v>
       </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
+      <c r="G8" s="1">
         <v>6.1979731122896231E-5</v>
       </c>
     </row>
@@ -2733,20 +2723,19 @@
       <c r="B9">
         <v>91</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>3.8346967576585424E-5</v>
       </c>
       <c r="D9">
         <v>258</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>8.5663314619108702E-5</v>
       </c>
       <c r="F9">
         <v>492</v>
       </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
+      <c r="G9" s="1">
         <v>6.7315734464602528E-5</v>
       </c>
     </row>
@@ -2757,20 +2746,19 @@
       <c r="B10">
         <v>111</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>4.6774872538472331E-5</v>
       </c>
       <c r="D10">
         <v>302</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>1.0027256207353033E-4</v>
       </c>
       <c r="F10">
         <v>575</v>
       </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
+      <c r="G10" s="1">
         <v>7.8671844140541572E-5</v>
       </c>
     </row>
@@ -2781,20 +2769,19 @@
       <c r="B11">
         <v>119</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>5.0146034523227095E-5</v>
       </c>
       <c r="D11">
         <v>278</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>9.2303881643845807E-5</v>
       </c>
       <c r="F11">
         <v>648</v>
       </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
+      <c r="G11" s="1">
         <v>8.8659747831427717E-5</v>
       </c>
     </row>
@@ -2805,20 +2792,19 @@
       <c r="B12">
         <v>132</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>5.5624172748453584E-5</v>
       </c>
       <c r="D12">
         <v>291</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>9.6620250209924929E-5</v>
       </c>
       <c r="F12">
         <v>718</v>
       </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
+      <c r="G12" s="1">
         <v>9.8237189726797994E-5</v>
       </c>
     </row>
@@ -2829,20 +2815,19 @@
       <c r="B13">
         <v>139</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>5.8573939485114002E-5</v>
       </c>
       <c r="D13">
         <v>317</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>1.0525298734208316E-4</v>
       </c>
       <c r="F13">
         <v>750</v>
       </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
+      <c r="G13" s="1">
         <v>1.0261544887896727E-4</v>
       </c>
     </row>
@@ -2853,20 +2838,19 @@
       <c r="B14">
         <v>135</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>5.6888358492736624E-5</v>
       </c>
       <c r="D14">
         <v>361</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>1.198622347965048E-4</v>
       </c>
       <c r="F14">
         <v>806</v>
       </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
+      <c r="G14" s="1">
         <v>1.1027740239526349E-4</v>
       </c>
     </row>
@@ -2877,20 +2861,19 @@
       <c r="B15">
         <v>155</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>6.5316263454623524E-5</v>
       </c>
       <c r="D15">
         <v>403</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>1.3380742554845273E-4</v>
       </c>
       <c r="F15">
         <v>917</v>
       </c>
-      <c r="G15">
-        <f t="shared" si="0"/>
+      <c r="G15" s="1">
         <v>1.2546448882935066E-4</v>
       </c>
     </row>
@@ -2901,20 +2884,19 @@
       <c r="B16">
         <v>168</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>7.0794401679850013E-5</v>
       </c>
       <c r="D16">
         <v>417</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>1.384558224657687E-4</v>
       </c>
       <c r="F16">
         <v>966</v>
       </c>
-      <c r="G16">
-        <f t="shared" si="0"/>
+      <c r="G16" s="1">
         <v>1.3216869815610983E-4</v>
       </c>
     </row>
@@ -2925,20 +2907,19 @@
       <c r="B17">
         <v>199</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>8.3857654370774723E-5</v>
       </c>
       <c r="D17">
         <v>427</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>1.4177610597813727E-4</v>
       </c>
       <c r="F17">
         <v>1024</v>
       </c>
-      <c r="G17">
-        <f t="shared" si="0"/>
+      <c r="G17" s="1">
         <v>1.4010429286941665E-4</v>
       </c>
     </row>
@@ -2949,20 +2930,19 @@
       <c r="B18">
         <v>206</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>8.6807421107435134E-5</v>
       </c>
       <c r="D18">
         <v>474</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>1.5738143848626946E-4</v>
       </c>
       <c r="F18">
         <v>1097</v>
       </c>
-      <c r="G18">
-        <f t="shared" si="0"/>
+      <c r="G18" s="1">
         <v>1.5009219656030278E-4</v>
       </c>
     </row>
@@ -2973,20 +2953,19 @@
       <c r="B19">
         <v>209</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>8.8071606851718173E-5</v>
       </c>
       <c r="D19">
         <v>521</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>1.7298677099440168E-4</v>
       </c>
       <c r="F19">
         <v>1191</v>
       </c>
-      <c r="G19">
-        <f t="shared" si="0"/>
+      <c r="G19" s="1">
         <v>1.6295333281980001E-4</v>
       </c>
     </row>
@@ -2997,20 +2976,19 @@
       <c r="B20">
         <v>216</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>9.1021373588378598E-5</v>
       </c>
       <c r="D20">
         <v>573</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <v>1.9025224525871814E-4</v>
       </c>
       <c r="F20">
         <v>1277</v>
       </c>
-      <c r="G20">
-        <f t="shared" si="0"/>
+      <c r="G20" s="1">
         <v>1.7471990429125493E-4</v>
       </c>
     </row>
@@ -3021,20 +2999,19 @@
       <c r="B21">
         <v>224</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>9.4392535573133355E-5</v>
       </c>
       <c r="D21">
         <v>628</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <v>2.0851380457674519E-4</v>
       </c>
       <c r="F21">
         <v>1470</v>
       </c>
-      <c r="G21">
-        <f t="shared" si="0"/>
+      <c r="G21" s="1">
         <v>2.0112627980277585E-4</v>
       </c>
     </row>
@@ -3045,20 +3022,19 @@
       <c r="B22">
         <v>251</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>1.0577020727168068E-4</v>
       </c>
       <c r="D22">
         <v>696</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="1">
         <v>2.3109173246085136E-4</v>
       </c>
       <c r="F22">
         <v>1571</v>
       </c>
-      <c r="G22">
-        <f t="shared" si="0"/>
+      <c r="G22" s="1">
         <v>2.1494516025181011E-4</v>
       </c>
     </row>
@@ -3069,20 +3045,19 @@
       <c r="B23">
         <v>270</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>1.1377671698547325E-4</v>
       </c>
       <c r="D23">
         <v>767</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="1">
         <v>2.5466574539866808E-4</v>
       </c>
       <c r="F23">
         <v>1743</v>
       </c>
-      <c r="G23">
-        <f t="shared" si="0"/>
+      <c r="G23" s="1">
         <v>2.3847830319471993E-4</v>
       </c>
     </row>
@@ -3093,20 +3068,19 @@
       <c r="B24">
         <v>300</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>1.2641857442830361E-4</v>
       </c>
       <c r="D24">
         <v>837</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="1">
         <v>2.7790772998524796E-4</v>
       </c>
       <c r="F24">
         <v>1996</v>
       </c>
-      <c r="G24">
-        <f t="shared" si="0"/>
+      <c r="G24" s="1">
         <v>2.7309391461655824E-4</v>
       </c>
     </row>
@@ -3117,20 +3091,19 @@
       <c r="B25">
         <v>366</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>1.5423066080253039E-4</v>
       </c>
       <c r="D25">
         <v>985</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1">
         <v>3.2704792596830259E-4</v>
       </c>
       <c r="F25">
         <v>2282</v>
       </c>
-      <c r="G25">
-        <f t="shared" si="0"/>
+      <c r="G25" s="1">
         <v>3.1222460578907109E-4</v>
       </c>
     </row>
@@ -3141,20 +3114,19 @@
       <c r="B26">
         <v>427</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>1.7993577093628545E-4</v>
       </c>
       <c r="D26">
         <v>1108</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1">
         <v>3.6788741317043581E-4</v>
       </c>
       <c r="F26">
         <v>2560</v>
       </c>
-      <c r="G26">
-        <f t="shared" si="0"/>
+      <c r="G26" s="1">
         <v>3.502607321735416E-4</v>
       </c>
     </row>
@@ -3165,20 +3137,19 @@
       <c r="B27">
         <v>523</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>2.2038971475334262E-4</v>
       </c>
       <c r="D27">
         <v>1190</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="1">
         <v>3.9511373797185794E-4</v>
       </c>
       <c r="F27">
         <v>2925</v>
       </c>
-      <c r="G27">
-        <f t="shared" si="0"/>
+      <c r="G27" s="1">
         <v>4.0020025062797234E-4</v>
       </c>
     </row>
@@ -3189,20 +3160,19 @@
       <c r="B28">
         <v>649</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>2.734855160132301E-4</v>
       </c>
       <c r="D28">
         <v>1302</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <v>4.3230091331038575E-4</v>
       </c>
       <c r="F28">
         <v>3287</v>
       </c>
-      <c r="G28">
-        <f t="shared" si="0"/>
+      <c r="G28" s="1">
         <v>4.4972930728688724E-4</v>
       </c>
     </row>
@@ -3213,20 +3183,19 @@
       <c r="B29">
         <v>748</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>3.1520364557457032E-4</v>
       </c>
       <c r="D29">
         <v>1475</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="1">
         <v>4.8974181807436175E-4</v>
       </c>
       <c r="F29">
         <v>3625</v>
       </c>
-      <c r="G29">
-        <f t="shared" si="0"/>
+      <c r="G29" s="1">
         <v>4.9597466958167509E-4</v>
       </c>
     </row>
@@ -3237,20 +3206,19 @@
       <c r="B30">
         <v>841</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>3.5439340364734444E-4</v>
       </c>
       <c r="D30">
         <v>1678</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="1">
         <v>5.5714357337544333E-4</v>
       </c>
       <c r="F30">
         <v>4215</v>
       </c>
-      <c r="G30">
-        <f t="shared" si="0"/>
+      <c r="G30" s="1">
         <v>5.7669882269979604E-4</v>
       </c>
     </row>
@@ -3261,20 +3229,19 @@
       <c r="B31">
         <v>1078</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>4.5426407744570427E-4</v>
       </c>
       <c r="D31">
         <v>1922</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="1">
         <v>6.3815849107723606E-4</v>
       </c>
       <c r="F31">
         <v>4851</v>
       </c>
-      <c r="G31">
-        <f t="shared" si="0"/>
+      <c r="G31" s="1">
         <v>6.6371672334916026E-4</v>
       </c>
     </row>
@@ -3285,20 +3252,19 @@
       <c r="B32">
         <v>1356</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <v>5.7141195641593231E-4</v>
       </c>
       <c r="D32">
         <v>2258</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="1">
         <v>7.4972001709281951E-4</v>
       </c>
       <c r="F32">
         <v>5542</v>
       </c>
-      <c r="G32">
-        <f t="shared" si="0"/>
+      <c r="G32" s="1">
         <v>7.5825975691631549E-4</v>
       </c>
     </row>
@@ -3309,20 +3275,19 @@
       <c r="B33">
         <v>1643</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <v>6.9235239261900938E-4</v>
       </c>
       <c r="D33">
         <v>2538</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="1">
         <v>8.42687955439139E-4</v>
       </c>
       <c r="F33">
         <v>6347</v>
       </c>
-      <c r="G33">
-        <f t="shared" si="0"/>
+      <c r="G33" s="1">
         <v>8.6840033871307361E-4</v>
       </c>
     </row>
@@ -3333,20 +3298,19 @@
       <c r="B34">
         <v>2060</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <v>8.6807421107435139E-4</v>
       </c>
       <c r="D34">
         <v>2779</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="1">
         <v>9.2270678808722116E-4</v>
       </c>
       <c r="F34">
         <v>7240</v>
       </c>
-      <c r="G34">
-        <f t="shared" si="0"/>
+      <c r="G34" s="1">
         <v>9.9058113317829731E-4</v>
       </c>
     </row>
@@ -3357,20 +3321,19 @@
       <c r="B35">
         <v>2529</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>1.0657085824305993E-3</v>
       </c>
       <c r="D35">
         <v>3132</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="1">
         <v>1.0399127960738312E-3</v>
       </c>
       <c r="F35">
         <v>8182</v>
       </c>
-      <c r="G35">
-        <f t="shared" si="0"/>
+      <c r="G35" s="1">
         <v>1.1194661369702803E-3</v>
       </c>
     </row>
@@ -3381,20 +3344,19 @@
       <c r="B36">
         <v>3072</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
         <v>1.2945262021458288E-3</v>
       </c>
       <c r="D36">
         <v>3678</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="1">
         <v>1.2212002758491543E-3</v>
       </c>
       <c r="F36">
         <v>9269</v>
       </c>
-      <c r="G36">
-        <f t="shared" si="0"/>
+      <c r="G36" s="1">
         <v>1.2681901275455301E-3</v>
       </c>
     </row>
@@ -3405,20 +3367,19 @@
       <c r="B37">
         <v>3555</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>1.4980601069753978E-3</v>
       </c>
       <c r="D37">
         <v>4125</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="1">
         <v>1.3696169488520286E-3</v>
       </c>
       <c r="F37">
         <v>10538</v>
       </c>
-      <c r="G37">
-        <f t="shared" si="0"/>
+      <c r="G37" s="1">
         <v>1.4418154670487427E-3</v>
       </c>
     </row>
@@ -3429,20 +3390,19 @@
       <c r="B38">
         <v>4277</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <v>1.802307476099515E-3</v>
       </c>
       <c r="D38">
         <v>4659</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="1">
         <v>1.5469200884125093E-3</v>
       </c>
       <c r="F38">
         <v>11833</v>
       </c>
-      <c r="G38">
-        <f t="shared" si="0"/>
+      <c r="G38" s="1">
         <v>1.618998142113093E-3</v>
       </c>
     </row>
@@ -3453,20 +3413,19 @@
       <c r="B39">
         <v>4961</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
         <v>2.0905418257960474E-3</v>
       </c>
       <c r="D39">
         <v>5249</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="1">
         <v>1.7428168156422542E-3</v>
       </c>
       <c r="F39">
         <v>13460</v>
       </c>
-      <c r="G39">
-        <f t="shared" si="0"/>
+      <c r="G39" s="1">
         <v>1.8416052558811993E-3</v>
       </c>
     </row>
@@ -3477,20 +3436,19 @@
       <c r="B40">
         <v>5814</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="1">
         <v>2.4499919724205238E-3</v>
       </c>
       <c r="D40">
         <v>5900</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="1">
         <v>1.958967272297447E-3</v>
       </c>
       <c r="F40">
         <v>15168</v>
       </c>
-      <c r="G40">
-        <f t="shared" si="0"/>
+      <c r="G40" s="1">
         <v>2.075294838128234E-3</v>
       </c>
     </row>
@@ -3501,20 +3459,19 @@
       <c r="B41">
         <v>6687</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="1">
         <v>2.8178700240068873E-3</v>
       </c>
       <c r="D41">
         <v>6628</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="1">
         <v>2.2006839119978775E-3</v>
       </c>
       <c r="F41">
         <v>17024</v>
       </c>
-      <c r="G41">
-        <f t="shared" si="0"/>
+      <c r="G41" s="1">
         <v>2.3292338689540515E-3</v>
       </c>
     </row>
@@ -3525,20 +3482,19 @@
       <c r="B42">
         <v>7734</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="1">
         <v>3.259070848761667E-3</v>
       </c>
       <c r="D42">
         <v>7251</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="1">
         <v>2.4075375748184385E-3</v>
       </c>
       <c r="F42">
         <v>18856</v>
       </c>
-      <c r="G42">
-        <f t="shared" si="0"/>
+      <c r="G42" s="1">
         <v>2.5798892054157423E-3</v>
       </c>
     </row>
@@ -3549,20 +3505,19 @@
       <c r="B43">
         <v>8641</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="1">
         <v>3.6412763387832382E-3</v>
       </c>
       <c r="D43">
         <v>8006</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="1">
         <v>2.6582189800022646E-3</v>
       </c>
       <c r="F43">
         <v>20663</v>
       </c>
-      <c r="G43">
-        <f t="shared" si="0"/>
+      <c r="G43" s="1">
         <v>2.827124026914801E-3</v>
       </c>
     </row>
@@ -3573,20 +3528,19 @@
       <c r="B44">
         <v>9444</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="1">
         <v>3.9796567230029976E-3</v>
       </c>
       <c r="D44">
         <v>8499</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="1">
         <v>2.8219089571620342E-3</v>
       </c>
       <c r="F44">
         <v>22014</v>
       </c>
-      <c r="G44">
-        <f t="shared" si="0"/>
+      <c r="G44" s="1">
         <v>3.0119686554954473E-3</v>
       </c>
     </row>
@@ -3597,20 +3551,19 @@
       <c r="B45">
         <v>10332</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="1">
         <v>4.3538557033107762E-3</v>
       </c>
       <c r="D45">
         <v>8840</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="1">
         <v>2.935130624933802E-3</v>
       </c>
       <c r="F45">
         <v>22675</v>
       </c>
-      <c r="G45">
-        <f t="shared" si="0"/>
+      <c r="G45" s="1">
         <v>3.1024070711074439E-3</v>
       </c>
     </row>
@@ -3621,20 +3574,19 @@
       <c r="B46">
         <v>10634</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="1">
         <v>4.4811170682352687E-3</v>
       </c>
       <c r="D46">
         <v>8498</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="1">
         <v>2.8215769288107975E-3</v>
       </c>
       <c r="F46">
         <v>22025</v>
       </c>
-      <c r="G46">
-        <f t="shared" si="0"/>
+      <c r="G46" s="1">
         <v>3.0134736820790053E-3</v>
       </c>
     </row>
@@ -3645,20 +3597,19 @@
       <c r="B47">
         <v>10256</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="1">
         <v>4.3218296644556061E-3</v>
       </c>
       <c r="D47">
         <v>7582</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="1">
         <v>2.5174389590778379E-3</v>
       </c>
       <c r="F47">
         <v>19838</v>
       </c>
-      <c r="G47">
-        <f t="shared" si="0"/>
+      <c r="G47" s="1">
         <v>2.714247033147937E-3</v>
       </c>
     </row>
@@ -3669,118 +3620,128 @@
       <c r="B48">
         <v>8912</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="1">
         <v>3.7554744510168055E-3</v>
       </c>
       <c r="D48">
         <v>6252</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="1">
         <v>2.0758412519328202E-3</v>
       </c>
       <c r="F48">
         <v>16135</v>
       </c>
-      <c r="G48">
-        <f t="shared" si="0"/>
+      <c r="G48" s="1">
         <v>2.2076003568828493E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>46</v>
       </c>
       <c r="B49">
         <v>6770</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="1">
         <v>2.852845829598718E-3</v>
       </c>
       <c r="D49">
         <v>4153</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="1">
         <v>1.3789137426866605E-3</v>
       </c>
       <c r="F49">
         <v>11212</v>
       </c>
-      <c r="G49">
-        <f t="shared" si="0"/>
+      <c r="G49" s="1">
         <v>1.534032550441308E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>47</v>
       </c>
       <c r="B50">
         <v>3835</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="1">
         <v>1.6160507764418144E-3</v>
       </c>
       <c r="D50">
         <v>2146</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="1">
         <v>7.1253284175429169E-4</v>
       </c>
       <c r="F50">
         <v>5954</v>
       </c>
-      <c r="G50">
-        <f t="shared" si="0"/>
+      <c r="G50" s="1">
         <v>8.146298435004948E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>48</v>
       </c>
       <c r="B51">
         <v>1345</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="1">
         <v>5.6677660868689446E-4</v>
       </c>
       <c r="D51">
         <v>708</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="1">
         <v>2.3507607267569364E-4</v>
       </c>
       <c r="F51">
         <v>1956</v>
       </c>
-      <c r="G51">
-        <f t="shared" si="0"/>
+      <c r="G51" s="1">
         <v>2.6762109067634664E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>49</v>
       </c>
       <c r="B52">
         <v>1</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="1">
         <v>4.2139524809434536E-7</v>
       </c>
       <c r="D52">
         <v>3</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="1">
         <v>9.9608505371056617E-7</v>
       </c>
       <c r="F52">
         <v>13</v>
       </c>
-      <c r="G52">
-        <f t="shared" si="0"/>
+      <c r="G52" s="1">
         <v>1.7786677805687659E-6</v>
       </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="H55" s="1"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="H56" s="1"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="H57" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3794,32 +3755,32 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -3836,13 +3797,13 @@
         <v>6.7</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -3859,13 +3820,13 @@
         <v>6.9</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -3882,10 +3843,10 @@
         <v>14.7</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -3902,10 +3863,10 @@
         <v>16.3</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -3922,10 +3883,10 @@
         <v>15.2</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -3942,13 +3903,13 @@
         <v>15.1</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -3965,13 +3926,13 @@
         <v>23.9</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -3988,13 +3949,13 @@
         <v>24.3</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
         <v>7</v>
-      </c>
-      <c r="G9" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -4011,13 +3972,13 @@
         <v>6.5</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -4034,13 +3995,13 @@
         <v>6.6</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -4057,10 +4018,10 @@
         <v>15.4</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -4077,10 +4038,10 @@
         <v>17.100000000000001</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -4097,10 +4058,10 @@
         <v>15.6</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -4117,13 +4078,13 @@
         <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -4140,13 +4101,13 @@
         <v>24.7</v>
       </c>
       <c r="E16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -4163,13 +4124,13 @@
         <v>25.1</v>
       </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
         <v>7</v>
-      </c>
-      <c r="G17" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -4186,13 +4147,13 @@
         <v>4.2</v>
       </c>
       <c r="E18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G18" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -4209,13 +4170,13 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F19" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G19" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -4232,10 +4193,10 @@
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -4252,10 +4213,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -4272,10 +4233,10 @@
         <v>12.5</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -4292,13 +4253,13 @@
         <v>15.6</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F23" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G23" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -4315,13 +4276,13 @@
         <v>20.100000000000001</v>
       </c>
       <c r="E24" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F24" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G24" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -4338,13 +4299,13 @@
         <v>20.6</v>
       </c>
       <c r="E25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" t="s">
         <v>7</v>
-      </c>
-      <c r="G25" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4354,9 +4315,6 @@
         <filter val="beam50"/>
       </filters>
     </filterColumn>
-    <sortState ref="A2:G25">
-      <sortCondition ref="E1:E25"/>
-    </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4374,182 +4332,182 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
         <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
         <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" t="s">
-        <v>35</v>
-      </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
         <v>39</v>
       </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
         <v>43</v>
       </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" t="s">
-        <v>46</v>
-      </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" t="s">
         <v>47</v>
       </c>
-      <c r="B8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" t="s">
-        <v>50</v>
-      </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>